<commit_message>
E355 HW4 Corrected values
</commit_message>
<xml_diff>
--- a/Stevens_Spring_2022/E-355-D/Homework/HW4/HW4.xlsx
+++ b/Stevens_Spring_2022/E-355-D/Homework/HW4/HW4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alex/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alex/Desktop/Stevens/Stevens_Spring_2022/E-355-D/Homework/HW4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEADB262-271A-1F49-9F78-3244F600CD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C4FD19-81DC-0245-81B0-BB06D4D2FE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{E0D2508D-8CCF-6545-9C15-05D38B4A77C0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E0D2508D-8CCF-6545-9C15-05D38B4A77C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -412,24 +412,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -470,15 +455,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -499,28 +475,52 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -628,7 +628,7 @@
             <c:v>Initial Cost</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -649,37 +649,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="25400" cap="rnd">
-                <a:noFill/>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-02AC-CD4F-BD07-D8DE37A08D0C}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
           <c:trendline>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
@@ -696,12 +665,12 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>[1]Sheet1!$B$3:$B$5</c:f>
+              <c:f>Sheet1!$B$23:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.18</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -714,18 +683,18 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>[1]Sheet1!$D$3:$D$5</c:f>
+              <c:f>Sheet1!$D$23:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12015200</c:v>
+                  <c:v>10132775</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12195200</c:v>
+                  <c:v>10282775</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12295200</c:v>
+                  <c:v>10382775</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -781,7 +750,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>[1]Sheet1!$B$7:$B$9</c:f>
+              <c:f>Sheet1!$B$27:$B$29</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -799,18 +768,18 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>[1]Sheet1!$D$7:$D$9</c:f>
+              <c:f>Sheet1!$D$27:$D$29</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15359000</c:v>
+                  <c:v>12979175</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12195200</c:v>
+                  <c:v>10282775</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10086000</c:v>
+                  <c:v>8485175</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2020,15 +1989,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>115729</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>87632</xdr:rowOff>
+      <xdr:colOff>569301</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>117870</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>11442</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>11442</xdr:rowOff>
+      <xdr:colOff>465014</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>41680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2419,8 +2388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D5C353-0CEE-004F-BAD2-E2254F41676C}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2435,22 +2404,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="48"/>
+      <c r="D1" s="48" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -2576,22 +2545,22 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13" t="s">
+      <c r="C10" s="48"/>
+      <c r="D10" s="48" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -2720,313 +2689,302 @@
     </row>
     <row r="20" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="18"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="44"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="20">
-        <v>0.18</v>
-      </c>
-      <c r="C23" s="21">
-        <v>1180000</v>
-      </c>
-      <c r="D23" s="21">
-        <v>12015200</v>
-      </c>
-      <c r="E23" s="22">
+      <c r="B23" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="C23" s="16">
+        <v>1150000</v>
+      </c>
+      <c r="D23" s="16">
+        <v>10132775</v>
+      </c>
+      <c r="E23" s="17">
         <f>D23-D24</f>
-        <v>-180000</v>
-      </c>
-      <c r="F23" s="23">
-        <f>E23/D24</f>
-        <v>-1.4759905536604567E-2</v>
-      </c>
-      <c r="I23" s="24">
-        <v>12195200</v>
-      </c>
+        <v>-150000</v>
+      </c>
+      <c r="F23" s="18">
+        <f>(E23/D24)</f>
+        <v>-1.4587501914609627E-2</v>
+      </c>
+      <c r="I23" s="19"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="26">
+      <c r="B24" s="21">
         <v>0</v>
       </c>
-      <c r="C24" s="24">
+      <c r="C24" s="19">
         <v>1000000</v>
       </c>
-      <c r="D24" s="24">
-        <v>12195200</v>
-      </c>
-      <c r="E24" s="27">
+      <c r="D24" s="19">
+        <v>10282775</v>
+      </c>
+      <c r="E24" s="22">
         <f>D24-D24</f>
         <v>0</v>
       </c>
-      <c r="F24" s="26" t="s">
+      <c r="F24" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="24">
-        <v>12195200</v>
-      </c>
+      <c r="I24" s="19"/>
     </row>
     <row r="25" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="29">
+      <c r="B25" s="24">
         <v>-0.1</v>
       </c>
-      <c r="C25" s="30">
+      <c r="C25" s="25">
         <v>900000</v>
       </c>
-      <c r="D25" s="30">
-        <v>12295200</v>
-      </c>
-      <c r="E25" s="31">
+      <c r="D25" s="25">
+        <v>10382775</v>
+      </c>
+      <c r="E25" s="26">
         <f>D25-D24</f>
         <v>100000</v>
       </c>
-      <c r="F25" s="32">
+      <c r="F25" s="27">
         <f>E25/D24</f>
-        <v>8.1999475203358707E-3</v>
-      </c>
-      <c r="I25" s="24">
-        <v>12195200</v>
-      </c>
+        <v>9.7250012764064173E-3</v>
+      </c>
+      <c r="I25" s="19"/>
     </row>
     <row r="26" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="35"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="47"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="36">
+      <c r="B27" s="28">
         <v>0.12</v>
       </c>
-      <c r="C27" s="21">
+      <c r="C27" s="16">
         <v>5600000</v>
       </c>
-      <c r="D27" s="21">
-        <v>15359000</v>
-      </c>
-      <c r="E27" s="22">
+      <c r="D27" s="16">
+        <v>12979175</v>
+      </c>
+      <c r="E27" s="17">
         <f>D27-D28</f>
-        <v>3163800</v>
-      </c>
-      <c r="F27" s="23">
+        <v>2696400</v>
+      </c>
+      <c r="F27" s="18">
         <f>E27/D28</f>
-        <v>0.25942993964838623</v>
+        <v>0.26222493441702266</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="26">
+      <c r="B28" s="21">
         <v>0</v>
       </c>
-      <c r="C28" s="24">
+      <c r="C28" s="19">
         <v>5000000</v>
       </c>
-      <c r="D28" s="24">
-        <v>12195200</v>
-      </c>
-      <c r="E28" s="27">
+      <c r="D28" s="19">
+        <f>D24</f>
+        <v>10282775</v>
+      </c>
+      <c r="E28" s="22">
         <f>D28-D28</f>
         <v>0</v>
       </c>
-      <c r="F28" s="25" t="s">
+      <c r="F28" s="20" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
+      <c r="A29" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="37">
+      <c r="B29" s="29">
         <v>-0.08</v>
       </c>
-      <c r="C29" s="30">
+      <c r="C29" s="25">
         <v>4600000</v>
       </c>
-      <c r="D29" s="30">
-        <v>10086000</v>
-      </c>
-      <c r="E29" s="31">
+      <c r="D29" s="25">
+        <v>8485175</v>
+      </c>
+      <c r="E29" s="26">
         <f>D29-D28</f>
-        <v>-2109200</v>
-      </c>
-      <c r="F29" s="32">
-        <f>E29/D28</f>
-        <v>-0.17295329309892415</v>
+        <v>-1797600</v>
+      </c>
+      <c r="F29" s="27">
+        <f>(E29/D28)</f>
+        <v>-0.17481662294468175</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F32" s="38"/>
+      <c r="F32" s="30"/>
     </row>
     <row r="33" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="39"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="31"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="20">
-        <v>0.18</v>
-      </c>
-      <c r="C34" s="40">
+      <c r="B34" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="C34" s="32">
         <f>F23</f>
-        <v>-1.4759905536604567E-2</v>
-      </c>
-      <c r="D34" s="41">
+        <v>-1.4587501914609627E-2</v>
+      </c>
+      <c r="D34" s="33">
         <f>ABS(C34/B34)</f>
-        <v>8.1999475203358707E-2</v>
-      </c>
-      <c r="E34" s="42" t="s">
+        <v>9.7250012764064184E-2</v>
+      </c>
+      <c r="E34" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="F34" s="43"/>
+      <c r="F34" s="34"/>
     </row>
     <row r="35" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="28" t="s">
+      <c r="A35" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="29">
+      <c r="B35" s="24">
         <v>-0.1</v>
       </c>
-      <c r="C35" s="44">
+      <c r="C35" s="35">
         <f>F25</f>
-        <v>8.1999475203358707E-3</v>
-      </c>
-      <c r="D35" s="45">
+        <v>9.7250012764064173E-3</v>
+      </c>
+      <c r="D35" s="36">
         <f>ABS(C35/B35)</f>
-        <v>8.1999475203358707E-2</v>
-      </c>
-      <c r="E35" s="46"/>
-      <c r="F35" s="47"/>
+        <v>9.725001276406417E-2</v>
+      </c>
+      <c r="E35" s="41"/>
+      <c r="F35" s="37"/>
     </row>
     <row r="36" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="33" t="s">
+      <c r="A36" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="43"/>
+      <c r="B36" s="46"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="34"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B37" s="36">
+      <c r="B37" s="28">
         <v>0.12</v>
       </c>
-      <c r="C37" s="40">
+      <c r="C37" s="32">
         <f>F27</f>
-        <v>0.25942993964838623</v>
-      </c>
-      <c r="D37" s="48">
+        <v>0.26222493441702266</v>
+      </c>
+      <c r="D37" s="38">
         <f>C37/B37</f>
-        <v>2.161916163736552</v>
-      </c>
-      <c r="E37" s="42" t="s">
+        <v>2.1852077868085225</v>
+      </c>
+      <c r="E37" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="39"/>
+      <c r="F37" s="31"/>
     </row>
     <row r="38" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="37">
+      <c r="B38" s="29">
         <v>-0.08</v>
       </c>
-      <c r="C38" s="44">
+      <c r="C38" s="35">
         <f>F29</f>
-        <v>-0.17295329309892415</v>
-      </c>
-      <c r="D38" s="45">
+        <v>-0.17481662294468175</v>
+      </c>
+      <c r="D38" s="36">
         <f>C38/B38</f>
-        <v>2.161916163736552</v>
-      </c>
-      <c r="E38" s="46"/>
-      <c r="F38" s="43"/>
+        <v>2.185207786808522</v>
+      </c>
+      <c r="E38" s="41"/>
+      <c r="F38" s="34"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F39" s="49"/>
+      <c r="F39" s="39"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F40" s="43"/>
+      <c r="F40" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="A36:E36"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -3035,6 +2993,12 @@
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="A36:E36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>